<commit_message>
Added vertical tail values
</commit_message>
<xml_diff>
--- a/Formal_Lab_Tom/Wind_Tunnel_Data.xlsx
+++ b/Formal_Lab_Tom/Wind_Tunnel_Data.xlsx
@@ -15,26 +15,39 @@
   </sheets>
   <definedNames>
     <definedName name="bspan">'Airplane Characteristics'!$C$5</definedName>
-    <definedName name="Cchord">'Airplane Characteristics'!$C$7</definedName>
-    <definedName name="CGw">'Airplane Characteristics'!$C$16</definedName>
+    <definedName name="Bval">'Airplane Characteristics'!$G$5</definedName>
+    <definedName name="Cchord">'Airplane Characteristics'!$C$8</definedName>
+    <definedName name="CGw">'Airplane Characteristics'!$C$22</definedName>
     <definedName name="Ct">'Airplane Characteristics'!$C$3</definedName>
-    <definedName name="lamda_t">'Airplane Characteristics'!$C$12</definedName>
+    <definedName name="flength">'Airplane Characteristics'!$C$34</definedName>
+    <definedName name="h_vt">'Airplane Characteristics'!$C$30</definedName>
+    <definedName name="l_vt">'Airplane Characteristics'!$C$31</definedName>
+    <definedName name="lamda_t">'Airplane Characteristics'!$C$16</definedName>
+    <definedName name="lamda_vt">'Airplane Characteristics'!$C$28</definedName>
     <definedName name="lamda_w">'Airplane Characteristics'!$C$6</definedName>
-    <definedName name="lbar">'Airplane Characteristics'!$C$17</definedName>
+    <definedName name="lbar">'Airplane Characteristics'!$C$23</definedName>
     <definedName name="NoModel65mph" localSheetId="3">'No Model 65 MPH'!$A$1:$M$75</definedName>
     <definedName name="nowind" localSheetId="0">'No wind'!$A$1:$H$70</definedName>
     <definedName name="Rc_">'Airplane Characteristics'!$C$4</definedName>
+    <definedName name="t_tail">'Airplane Characteristics'!$C$17</definedName>
+    <definedName name="t_wing">'Airplane Characteristics'!$C$7</definedName>
     <definedName name="tailoff65mph" localSheetId="2">'Tail OFf 65 MPH'!$A$1:$H$76</definedName>
     <definedName name="tailon65mph" localSheetId="1">'Tail On 65 MPH'!$A$1:$H$85</definedName>
-    <definedName name="tamc">'Airplane Characteristics'!$C$15</definedName>
-    <definedName name="tmac">'Airplane Characteristics'!$C$15</definedName>
-    <definedName name="Trc">'Airplane Characteristics'!$C$10</definedName>
-    <definedName name="Ttc">'Airplane Characteristics'!$C$11</definedName>
+    <definedName name="tamc">'Airplane Characteristics'!$C$21</definedName>
+    <definedName name="tau1_">'Airplane Characteristics'!$G$6</definedName>
+    <definedName name="tmac">'Airplane Characteristics'!$C$21</definedName>
+    <definedName name="Trc">'Airplane Characteristics'!$C$14</definedName>
+    <definedName name="Ttc">'Airplane Characteristics'!$C$15</definedName>
     <definedName name="TunHeight">'Airplane Characteristics'!$G$3</definedName>
     <definedName name="TunLen">'Airplane Characteristics'!$G$4</definedName>
     <definedName name="TunWidth">'Airplane Characteristics'!$G$2</definedName>
-    <definedName name="wing_area">'Airplane Characteristics'!$C$8</definedName>
-    <definedName name="wmac">'Airplane Characteristics'!$C$14</definedName>
+    <definedName name="vol_tail">'Airplane Characteristics'!$C$19</definedName>
+    <definedName name="vol_wing">'Airplane Characteristics'!$C$10</definedName>
+    <definedName name="vtMAC">'Airplane Characteristics'!$C$29</definedName>
+    <definedName name="vtRc">'Airplane Characteristics'!$C$26</definedName>
+    <definedName name="vtTc">'Airplane Characteristics'!$C$27</definedName>
+    <definedName name="wing_area">'Airplane Characteristics'!$C$9</definedName>
+    <definedName name="wmac">'Airplane Characteristics'!$C$20</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -80,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="75">
   <si>
     <t>Alpha (deg)</t>
   </si>
@@ -178,9 +191,6 @@
     <t>Parameter</t>
   </si>
   <si>
-    <t>Airplane Characteristics</t>
-  </si>
-  <si>
     <t>Tail MAC (in)</t>
   </si>
   <si>
@@ -231,13 +241,92 @@
   <si>
     <t>TunLen</t>
   </si>
+  <si>
+    <t xml:space="preserve">B Value </t>
+  </si>
+  <si>
+    <t>Bval</t>
+  </si>
+  <si>
+    <t>tau1</t>
+  </si>
+  <si>
+    <t>Correction Factors</t>
+  </si>
+  <si>
+    <t>Fuselage Characteristics</t>
+  </si>
+  <si>
+    <t>flength</t>
+  </si>
+  <si>
+    <t>Tail Thickness</t>
+  </si>
+  <si>
+    <t>t_tail</t>
+  </si>
+  <si>
+    <t>Tail Volume (in^3)</t>
+  </si>
+  <si>
+    <t>vol_tail</t>
+  </si>
+  <si>
+    <t>Wing Thickness (in)</t>
+  </si>
+  <si>
+    <t>t_wing</t>
+  </si>
+  <si>
+    <t>Wing Volume (in^3)</t>
+  </si>
+  <si>
+    <t>vol_wing</t>
+  </si>
+  <si>
+    <t>Horizontal Tail Characteristics</t>
+  </si>
+  <si>
+    <t>Wing Characteristics</t>
+  </si>
+  <si>
+    <t>Vertical Tail Characteristics</t>
+  </si>
+  <si>
+    <t>vtRc</t>
+  </si>
+  <si>
+    <t>Tip Chord</t>
+  </si>
+  <si>
+    <t>vtTc</t>
+  </si>
+  <si>
+    <t>MAC (in)</t>
+  </si>
+  <si>
+    <t>vtMAC</t>
+  </si>
+  <si>
+    <t>lamda_vt</t>
+  </si>
+  <si>
+    <t>h_vt</t>
+  </si>
+  <si>
+    <t>l_vt</t>
+  </si>
+  <si>
+    <t>Extrapolated Length (in)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="0.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -270,7 +359,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -293,11 +382,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -307,7 +405,15 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8982,15 +9088,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
@@ -8998,12 +9104,12 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
       <c r="E1" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -9019,10 +9125,10 @@
         <v>29</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G2" s="3">
         <v>40</v>
@@ -9039,10 +9145,10 @@
         <v>1.2889999999999999</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>47</v>
       </c>
       <c r="G3" s="3">
         <v>28</v>
@@ -9059,10 +9165,10 @@
         <v>2.5790000000000002</v>
       </c>
       <c r="E4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>49</v>
       </c>
       <c r="G4" s="3">
         <v>54</v>
@@ -9076,11 +9182,19 @@
         <v>23</v>
       </c>
       <c r="C5" s="3">
-        <v>60</v>
-      </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
+        <f>24+3/8</f>
+        <v>24.375</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G5" s="7">
+        <f>TunWidth/TunHeight</f>
+        <v>1.4285714285714286</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
@@ -9093,174 +9207,371 @@
         <f>Ct/Rc_</f>
         <v>0.49980612640558347</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
+      <c r="E6" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0.85499999999999998</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.35</v>
+      </c>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="8"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C8" s="1">
         <f>(Rc_/28)*30</f>
         <v>2.7632142857142856</v>
       </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="5">
-        <f>0.5*(Cchord+Ct)*bspan</f>
-        <v>121.56642857142856</v>
-      </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="5">
+        <f>0.5*(Cchord+Ct)*bspan</f>
+        <v>49.386361607142852</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" s="4">
+        <f>wing_area*t_wing</f>
+        <v>17.285226562499997</v>
+      </c>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C11" s="4">
         <f>bspan^2/wing_area</f>
-        <v>29.613438860587689</v>
-      </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+        <v>12.030459537113748</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C14" s="3">
         <v>1.75</v>
       </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B15" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C15" s="3">
         <v>1</v>
       </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" s="3">
+      <c r="C16" s="3">
         <f>Ttc/Trc</f>
         <v>0.5714285714285714</v>
       </c>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="3">
+        <v>0.17</v>
+      </c>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B18" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C18" s="1">
         <f>(Ttc+Trc)*2.75</f>
         <v>7.5625</v>
       </c>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" s="1">
+        <f>C18*t_tail</f>
+        <v>1.285625</v>
+      </c>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" s="1">
+      <c r="C20" s="1">
         <f>(2*Rc_)/3*((1+lamda_w+lamda_w^2)/(1+lamda_w))</f>
         <v>2.0057037228541885</v>
       </c>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" s="1">
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="1">
         <f>(2*Trc)/3*((1+lamda_t+lamda_t^2)/(1+lamda_t))</f>
         <v>1.4090909090909089</v>
       </c>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C16" s="1">
+      <c r="C22" s="1">
         <f>0.25*wmac</f>
         <v>0.50142593071354713</v>
       </c>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C17" s="3"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
+      <c r="C23" s="3"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C26" s="3">
+        <v>2.95</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C27" s="3">
+        <v>1.95</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C28" s="7">
+        <f>vtTc/vtRc</f>
+        <v>0.66101694915254228</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C29" s="7">
+        <f>(2*vtRc)/3*((1+lamda_vt+lamda_vt^2)/(1+lamda_vt))</f>
+        <v>2.4840136054421769</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C30" s="3">
+        <v>2.15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C31" s="3">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="8"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="8"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C34" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="3"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="3"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="8"/>
+      <c r="B40" s="8"/>
+      <c r="C40" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="6">
+    <mergeCell ref="A33:C33"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="E1:G1"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A25:C25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added correction Cls and Cds
</commit_message>
<xml_diff>
--- a/Formal_Lab_Tom/Wind_Tunnel_Data.xlsx
+++ b/Formal_Lab_Tom/Wind_Tunnel_Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="No wind" sheetId="1" r:id="rId1"/>
@@ -115,7 +115,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="121">
   <si>
     <t>Alpha (deg)</t>
   </si>
@@ -470,6 +470,15 @@
   <si>
     <t>eps_tot_nt</t>
   </si>
+  <si>
+    <t>Dynamic Pressure (Corrected)</t>
+  </si>
+  <si>
+    <t>CL (corrected)</t>
+  </si>
+  <si>
+    <t>CD (corrected)</t>
+  </si>
 </sst>
 </file>
 
@@ -557,7 +566,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -575,6 +584,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4162,10 +4172,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K85"/>
+  <dimension ref="A1:N85"/>
   <sheetViews>
-    <sheetView topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:K85"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4178,9 +4188,12 @@
     <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4214,8 +4227,17 @@
       <c r="K1" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" t="s">
+        <v>118</v>
+      </c>
+      <c r="M1" t="s">
+        <v>119</v>
+      </c>
+      <c r="N1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>-4.7E-2</v>
       </c>
@@ -4253,8 +4275,20 @@
         <f>I2^2</f>
         <v>1.2584357375224169E-8</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M2">
+        <f>B2/(L2*wing_area)</f>
+        <v>1.1143478347379423E-4</v>
+      </c>
+      <c r="N2">
+        <f>D2/(L2*wing_area)</f>
+        <v>2.5786331572692774E-5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>-4.7E-2</v>
       </c>
@@ -4292,8 +4326,20 @@
         <f t="shared" ref="K3:K66" si="1">I3^2</f>
         <v>1.2584357375224169E-8</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M3">
+        <f>B3/(L3*wing_area)</f>
+        <v>1.1143478347379423E-4</v>
+      </c>
+      <c r="N3">
+        <f>D3/(L3*wing_area)</f>
+        <v>2.5786331572692774E-5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>-4.7E-2</v>
       </c>
@@ -4331,8 +4377,20 @@
         <f t="shared" si="1"/>
         <v>1.2584357375224169E-8</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M4">
+        <f>B4/(L4*wing_area)</f>
+        <v>1.1143478347379423E-4</v>
+      </c>
+      <c r="N4">
+        <f>D4/(L4*wing_area)</f>
+        <v>2.5786331572692774E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>-4.7E-2</v>
       </c>
@@ -4370,8 +4428,20 @@
         <f t="shared" si="1"/>
         <v>1.2584357375224169E-8</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M5">
+        <f>B5/(L5*wing_area)</f>
+        <v>1.1143478347379423E-4</v>
+      </c>
+      <c r="N5">
+        <f>D5/(L5*wing_area)</f>
+        <v>2.5786331572692774E-5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>-4.2000000000000003E-2</v>
       </c>
@@ -4409,8 +4479,20 @@
         <f t="shared" si="1"/>
         <v>1.2527876101835618E-8</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M6">
+        <f>B6/(L6*wing_area)</f>
+        <v>1.1118443074007875E-4</v>
+      </c>
+      <c r="N6">
+        <f>D6/(L6*wing_area)</f>
+        <v>2.4117313347923014E-5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>-4.7E-2</v>
       </c>
@@ -4448,8 +4530,20 @@
         <f t="shared" si="1"/>
         <v>1.3002435012007012E-8</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M7">
+        <f>B7/(L7*wing_area)</f>
+        <v>1.1327070352104096E-4</v>
+      </c>
+      <c r="N7">
+        <f>D7/(L7*wing_area)</f>
+        <v>2.4812737608243746E-5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>-4.7E-2</v>
       </c>
@@ -4487,8 +4581,20 @@
         <f t="shared" si="1"/>
         <v>1.3002435012007012E-8</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L8" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M8">
+        <f>B8/(L8*wing_area)</f>
+        <v>1.1327070352104096E-4</v>
+      </c>
+      <c r="N8">
+        <f>D8/(L8*wing_area)</f>
+        <v>2.4812737608243746E-5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>-4.7E-2</v>
       </c>
@@ -4526,8 +4632,20 @@
         <f t="shared" si="1"/>
         <v>1.3002435012007012E-8</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M9">
+        <f>B9/(L9*wing_area)</f>
+        <v>1.1327070352104096E-4</v>
+      </c>
+      <c r="N9">
+        <f>D9/(L9*wing_area)</f>
+        <v>2.4812737608243746E-5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>-4.7E-2</v>
       </c>
@@ -4565,8 +4683,20 @@
         <f t="shared" si="1"/>
         <v>1.3002435012007012E-8</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L10" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M10">
+        <f>B10/(L10*wing_area)</f>
+        <v>1.1327070352104096E-4</v>
+      </c>
+      <c r="N10">
+        <f>D10/(L10*wing_area)</f>
+        <v>2.4812737608243746E-5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>-4.4999999999999998E-2</v>
       </c>
@@ -4604,8 +4734,20 @@
         <f t="shared" si="1"/>
         <v>1.4170701929633841E-8</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L11" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M11">
+        <f>B11/(L11*wing_area)</f>
+        <v>1.1824994122493741E-4</v>
+      </c>
+      <c r="N11">
+        <f>D11/(L11*wing_area)</f>
+        <v>2.4784920637830915E-5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>-4.5999999999999999E-2</v>
       </c>
@@ -4643,8 +4785,20 @@
         <f t="shared" si="1"/>
         <v>9.0543213097676161E-9</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L12" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M12">
+        <f>B12/(L12*wing_area)</f>
+        <v>9.4522065462794E-5</v>
+      </c>
+      <c r="N12">
+        <f>D12/(L12*wing_area)</f>
+        <v>2.2615196945630227E-5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>-4.7E-2</v>
       </c>
@@ -4682,8 +4836,20 @@
         <f t="shared" si="1"/>
         <v>1.1263868536527303E-8</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L13" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M13">
+        <f>B13/(L13*wing_area)</f>
+        <v>1.0542631786462309E-4</v>
+      </c>
+      <c r="N13">
+        <f>D13/(L13*wing_area)</f>
+        <v>2.6287037040123699E-5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>-4.7E-2</v>
       </c>
@@ -4721,8 +4887,20 @@
         <f t="shared" si="1"/>
         <v>1.1263868536527303E-8</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L14" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M14">
+        <f>B14/(L14*wing_area)</f>
+        <v>1.0542631786462309E-4</v>
+      </c>
+      <c r="N14">
+        <f>D14/(L14*wing_area)</f>
+        <v>2.6287037040123699E-5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>-4.7E-2</v>
       </c>
@@ -4760,8 +4938,20 @@
         <f t="shared" si="1"/>
         <v>1.1263868536527303E-8</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L15" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M15">
+        <f>B15/(L15*wing_area)</f>
+        <v>1.0542631786462309E-4</v>
+      </c>
+      <c r="N15">
+        <f>D15/(L15*wing_area)</f>
+        <v>2.6287037040123699E-5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>-4.7E-2</v>
       </c>
@@ -4799,8 +4989,20 @@
         <f t="shared" si="1"/>
         <v>1.1263868536527303E-8</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L16" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M16">
+        <f>B16/(L16*wing_area)</f>
+        <v>1.0542631786462309E-4</v>
+      </c>
+      <c r="N16">
+        <f>D16/(L16*wing_area)</f>
+        <v>2.6287037040123699E-5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>-8.0860000000000003</v>
       </c>
@@ -4838,8 +5040,20 @@
         <f t="shared" si="1"/>
         <v>5.8402406736801484E-10</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L17" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M17">
+        <f>B17/(L17*wing_area)</f>
+        <v>2.4006045466271695E-5</v>
+      </c>
+      <c r="N17">
+        <f>D17/(L17*wing_area)</f>
+        <v>1.972223202269598E-5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>-8.0860000000000003</v>
       </c>
@@ -4877,8 +5091,20 @@
         <f t="shared" si="1"/>
         <v>5.8402406736801484E-10</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L18" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M18">
+        <f>B18/(L18*wing_area)</f>
+        <v>2.4006045466271695E-5</v>
+      </c>
+      <c r="N18">
+        <f>D18/(L18*wing_area)</f>
+        <v>1.972223202269598E-5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>-8.0860000000000003</v>
       </c>
@@ -4916,8 +5142,20 @@
         <f t="shared" si="1"/>
         <v>5.8402406736801484E-10</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L19" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M19">
+        <f>B19/(L19*wing_area)</f>
+        <v>2.4006045466271695E-5</v>
+      </c>
+      <c r="N19">
+        <f>D19/(L19*wing_area)</f>
+        <v>1.972223202269598E-5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>-8.0860000000000003</v>
       </c>
@@ -4955,8 +5193,20 @@
         <f t="shared" si="1"/>
         <v>5.8402406736801484E-10</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L20" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M20">
+        <f>B20/(L20*wing_area)</f>
+        <v>2.4006045466271695E-5</v>
+      </c>
+      <c r="N20">
+        <f>D20/(L20*wing_area)</f>
+        <v>1.972223202269598E-5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>-8.0860000000000003</v>
       </c>
@@ -4994,8 +5244,20 @@
         <f t="shared" si="1"/>
         <v>5.8402406736801484E-10</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L21" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M21">
+        <f>B21/(L21*wing_area)</f>
+        <v>2.4006045466271695E-5</v>
+      </c>
+      <c r="N21">
+        <f>D21/(L21*wing_area)</f>
+        <v>1.972223202269598E-5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>-6.0060000000000002</v>
       </c>
@@ -5033,8 +5295,20 @@
         <f t="shared" si="1"/>
         <v>2.8159671341318259E-9</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L22" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M22">
+        <f>B22/(L22*wing_area)</f>
+        <v>5.2713158932311547E-5</v>
+      </c>
+      <c r="N22">
+        <f>D22/(L22*wing_area)</f>
+        <v>2.3254987265125305E-5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>-6.0060000000000002</v>
       </c>
@@ -5072,8 +5346,20 @@
         <f t="shared" si="1"/>
         <v>2.8159671341318259E-9</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L23" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M23">
+        <f>B23/(L23*wing_area)</f>
+        <v>5.2713158932311547E-5</v>
+      </c>
+      <c r="N23">
+        <f>D23/(L23*wing_area)</f>
+        <v>2.3254987265125305E-5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>-6.0060000000000002</v>
       </c>
@@ -5111,8 +5397,20 @@
         <f t="shared" si="1"/>
         <v>2.8159671341318259E-9</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L24" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M24">
+        <f>B24/(L24*wing_area)</f>
+        <v>5.2713158932311547E-5</v>
+      </c>
+      <c r="N24">
+        <f>D24/(L24*wing_area)</f>
+        <v>2.3254987265125305E-5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>-6.0060000000000002</v>
       </c>
@@ -5150,8 +5448,20 @@
         <f t="shared" si="1"/>
         <v>2.8159671341318259E-9</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L25" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M25">
+        <f>B25/(L25*wing_area)</f>
+        <v>5.2713158932311547E-5</v>
+      </c>
+      <c r="N25">
+        <f>D25/(L25*wing_area)</f>
+        <v>2.3254987265125305E-5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>-6.0060000000000002</v>
       </c>
@@ -5189,8 +5499,20 @@
         <f t="shared" si="1"/>
         <v>2.8159671341318259E-9</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L26" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M26">
+        <f>B26/(L26*wing_area)</f>
+        <v>5.2713158932311547E-5</v>
+      </c>
+      <c r="N26">
+        <f>D26/(L26*wing_area)</f>
+        <v>2.3254987265125305E-5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>-3.9950000000000001</v>
       </c>
@@ -5228,8 +5550,20 @@
         <f t="shared" si="1"/>
         <v>3.9241095335290972E-9</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L27" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M27">
+        <f>B27/(L27*wing_area)</f>
+        <v>6.2226562813499171E-5</v>
+      </c>
+      <c r="N27">
+        <f>D27/(L27*wing_area)</f>
+        <v>2.2197942389437792E-5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>-3.9950000000000001</v>
       </c>
@@ -5267,8 +5601,20 @@
         <f t="shared" si="1"/>
         <v>4.8151714710040527E-9</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L28" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M28">
+        <f>B28/(L28*wing_area)</f>
+        <v>6.8930452682991033E-5</v>
+      </c>
+      <c r="N28">
+        <f>D28/(L28*wing_area)</f>
+        <v>2.105744660251179E-5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>-3.9950000000000001</v>
       </c>
@@ -5306,8 +5652,20 @@
         <f t="shared" si="1"/>
         <v>4.8151714710040527E-9</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L29" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M29">
+        <f>B29/(L29*wing_area)</f>
+        <v>6.8930452682991033E-5</v>
+      </c>
+      <c r="N29">
+        <f>D29/(L29*wing_area)</f>
+        <v>2.105744660251179E-5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>-3.9950000000000001</v>
       </c>
@@ -5345,8 +5703,20 @@
         <f t="shared" si="1"/>
         <v>4.8151714710040527E-9</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L30" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M30">
+        <f>B30/(L30*wing_area)</f>
+        <v>6.8930452682991033E-5</v>
+      </c>
+      <c r="N30">
+        <f>D30/(L30*wing_area)</f>
+        <v>2.105744660251179E-5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>-3.9950000000000001</v>
       </c>
@@ -5384,8 +5754,20 @@
         <f t="shared" si="1"/>
         <v>4.8151714710040527E-9</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L31" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M31">
+        <f>B31/(L31*wing_area)</f>
+        <v>6.8930452682991033E-5</v>
+      </c>
+      <c r="N31">
+        <f>D31/(L31*wing_area)</f>
+        <v>2.105744660251179E-5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>-2.0299999999999998</v>
       </c>
@@ -5423,8 +5805,20 @@
         <f t="shared" si="1"/>
         <v>7.7069802039397532E-9</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L32" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M32">
+        <f>B32/(L32*wing_area)</f>
+        <v>8.7206202244219884E-5</v>
+      </c>
+      <c r="N32">
+        <f>D32/(L32*wing_area)</f>
+        <v>1.911025867361374E-5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>-2.0299999999999998</v>
       </c>
@@ -5462,8 +5856,20 @@
         <f t="shared" si="1"/>
         <v>7.7069802039397532E-9</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L33" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M33">
+        <f>B33/(L33*wing_area)</f>
+        <v>8.7206202244219884E-5</v>
+      </c>
+      <c r="N33">
+        <f>D33/(L33*wing_area)</f>
+        <v>1.911025867361374E-5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>-1.976</v>
       </c>
@@ -5501,8 +5907,20 @@
         <f t="shared" si="1"/>
         <v>8.7950729941904794E-9</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L34" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M34">
+        <f>B34/(L34*wing_area)</f>
+        <v>9.3159033912565363E-5</v>
+      </c>
+      <c r="N34">
+        <f>D34/(L34*wing_area)</f>
+        <v>2.3115902413061155E-5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>-1.976</v>
       </c>
@@ -5540,8 +5958,20 @@
         <f t="shared" si="1"/>
         <v>8.7950729941904794E-9</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L35" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M35">
+        <f>B35/(L35*wing_area)</f>
+        <v>9.3159033912565363E-5</v>
+      </c>
+      <c r="N35">
+        <f>D35/(L35*wing_area)</f>
+        <v>2.3115902413061155E-5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>-1.976</v>
       </c>
@@ -5579,8 +6009,20 @@
         <f t="shared" si="1"/>
         <v>8.7950729941904794E-9</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L36" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M36">
+        <f>B36/(L36*wing_area)</f>
+        <v>9.3159033912565363E-5</v>
+      </c>
+      <c r="N36">
+        <f>D36/(L36*wing_area)</f>
+        <v>2.3115902413061155E-5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>1.9E-2</v>
       </c>
@@ -5618,8 +6060,20 @@
         <f t="shared" si="1"/>
         <v>9.865782346723716E-9</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L37" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M37">
+        <f>B37/(L37*wing_area)</f>
+        <v>9.8666794054305578E-5</v>
+      </c>
+      <c r="N37">
+        <f>D37/(L37*wing_area)</f>
+        <v>2.6287037040123699E-5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>1.9E-2</v>
       </c>
@@ -5657,8 +6111,20 @@
         <f t="shared" si="1"/>
         <v>9.865782346723716E-9</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L38" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M38">
+        <f>B38/(L38*wing_area)</f>
+        <v>9.8666794054305578E-5</v>
+      </c>
+      <c r="N38">
+        <f>D38/(L38*wing_area)</f>
+        <v>2.6287037040123699E-5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>1.9E-2</v>
       </c>
@@ -5696,8 +6162,20 @@
         <f t="shared" si="1"/>
         <v>9.865782346723716E-9</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L39" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M39">
+        <f>B39/(L39*wing_area)</f>
+        <v>9.8666794054305578E-5</v>
+      </c>
+      <c r="N39">
+        <f>D39/(L39*wing_area)</f>
+        <v>2.6287037040123699E-5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>1.9E-2</v>
       </c>
@@ -5735,8 +6213,20 @@
         <f t="shared" si="1"/>
         <v>9.865782346723716E-9</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L40" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M40">
+        <f>B40/(L40*wing_area)</f>
+        <v>9.8666794054305578E-5</v>
+      </c>
+      <c r="N40">
+        <f>D40/(L40*wing_area)</f>
+        <v>2.6287037040123699E-5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>1.9E-2</v>
       </c>
@@ -5774,8 +6264,20 @@
         <f t="shared" si="1"/>
         <v>9.865782346723716E-9</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L41" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M41">
+        <f>B41/(L41*wing_area)</f>
+        <v>9.8666794054305578E-5</v>
+      </c>
+      <c r="N41">
+        <f>D41/(L41*wing_area)</f>
+        <v>2.6287037040123699E-5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>1.992</v>
       </c>
@@ -5813,8 +6315,20 @@
         <f t="shared" si="1"/>
         <v>1.6070527863160038E-8</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L42" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M42">
+        <f>B42/(L42*wing_area)</f>
+        <v>1.259274250588783E-4</v>
+      </c>
+      <c r="N42">
+        <f>D42/(L42*wing_area)</f>
+        <v>2.7705702531177993E-5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>1.992</v>
       </c>
@@ -5852,8 +6366,20 @@
         <f t="shared" si="1"/>
         <v>1.6070527863160038E-8</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L43" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M43">
+        <f>B43/(L43*wing_area)</f>
+        <v>1.259274250588783E-4</v>
+      </c>
+      <c r="N43">
+        <f>D43/(L43*wing_area)</f>
+        <v>2.7705702531177993E-5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>1.99</v>
       </c>
@@ -5891,8 +6417,20 @@
         <f t="shared" si="1"/>
         <v>1.5181493784307306E-8</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L44" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M44">
+        <f>B44/(L44*wing_area)</f>
+        <v>1.2239466981644898E-4</v>
+      </c>
+      <c r="N44">
+        <f>D44/(L44*wing_area)</f>
+        <v>3.0209229868332636E-5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>1.99</v>
       </c>
@@ -5930,8 +6468,20 @@
         <f t="shared" si="1"/>
         <v>1.5181493784307306E-8</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L45" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M45">
+        <f>B45/(L45*wing_area)</f>
+        <v>1.2239466981644898E-4</v>
+      </c>
+      <c r="N45">
+        <f>D45/(L45*wing_area)</f>
+        <v>3.0209229868332636E-5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>1.99</v>
       </c>
@@ -5969,8 +6519,20 @@
         <f t="shared" si="1"/>
         <v>1.5181493784307306E-8</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L46" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M46">
+        <f>B46/(L46*wing_area)</f>
+        <v>1.2239466981644898E-4</v>
+      </c>
+      <c r="N46">
+        <f>D46/(L46*wing_area)</f>
+        <v>3.0209229868332636E-5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>3.9750000000000001</v>
       </c>
@@ -6008,8 +6570,20 @@
         <f t="shared" si="1"/>
         <v>2.2018969615112213E-8</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L47" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M47">
+        <f>B47/(L47*wing_area)</f>
+        <v>1.4740212621758254E-4</v>
+      </c>
+      <c r="N47">
+        <f>D47/(L47*wing_area)</f>
+        <v>3.2406770530946151E-5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>3.9750000000000001</v>
       </c>
@@ -6047,8 +6621,20 @@
         <f t="shared" si="1"/>
         <v>2.2018969615112213E-8</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L48" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M48">
+        <f>B48/(L48*wing_area)</f>
+        <v>1.4740212621758254E-4</v>
+      </c>
+      <c r="N48">
+        <f>D48/(L48*wing_area)</f>
+        <v>3.2406770530946151E-5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>4.0259999999999998</v>
       </c>
@@ -6086,8 +6672,20 @@
         <f t="shared" si="1"/>
         <v>2.3755599979633578E-8</v>
       </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L49" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M49">
+        <f>B49/(L49*wing_area)</f>
+        <v>1.5310460515221251E-4</v>
+      </c>
+      <c r="N49">
+        <f>D49/(L49*wing_area)</f>
+        <v>3.5383186365118883E-5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>4.0259999999999998</v>
       </c>
@@ -6125,8 +6723,20 @@
         <f t="shared" si="1"/>
         <v>2.3755599979633578E-8</v>
       </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L50" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M50">
+        <f>B50/(L50*wing_area)</f>
+        <v>1.5310460515221251E-4</v>
+      </c>
+      <c r="N50">
+        <f>D50/(L50*wing_area)</f>
+        <v>3.5383186365118883E-5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>4.0259999999999998</v>
       </c>
@@ -6164,8 +6774,20 @@
         <f t="shared" si="1"/>
         <v>2.3755599979633578E-8</v>
       </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L51" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M51">
+        <f>B51/(L51*wing_area)</f>
+        <v>1.5310460515221251E-4</v>
+      </c>
+      <c r="N51">
+        <f>D51/(L51*wing_area)</f>
+        <v>3.5383186365118883E-5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>6.0010000000000003</v>
       </c>
@@ -6203,8 +6825,20 @@
         <f t="shared" si="1"/>
         <v>2.9006944549743138E-8</v>
       </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L52" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M52">
+        <f>B52/(L52*wing_area)</f>
+        <v>1.6918281405082787E-4</v>
+      </c>
+      <c r="N52">
+        <f>D52/(L52*wing_area)</f>
+        <v>4.3227572021536751E-5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>6.0149999999999997</v>
       </c>
@@ -6242,8 +6876,20 @@
         <f t="shared" si="1"/>
         <v>2.5899509986650089E-8</v>
       </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L53" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M53">
+        <f>B53/(L53*wing_area)</f>
+        <v>1.5986412896253004E-4</v>
+      </c>
+      <c r="N53">
+        <f>D53/(L53*wing_area)</f>
+        <v>4.1586370767179821E-5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>6.0149999999999997</v>
       </c>
@@ -6281,8 +6927,20 @@
         <f t="shared" si="1"/>
         <v>2.5899509986650089E-8</v>
       </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L54" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M54">
+        <f>B54/(L54*wing_area)</f>
+        <v>1.5986412896253004E-4</v>
+      </c>
+      <c r="N54">
+        <f>D54/(L54*wing_area)</f>
+        <v>4.1586370767179821E-5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>6.0149999999999997</v>
       </c>
@@ -6320,8 +6978,20 @@
         <f t="shared" si="1"/>
         <v>2.5899509986650089E-8</v>
       </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L55" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M55">
+        <f>B55/(L55*wing_area)</f>
+        <v>1.5986412896253004E-4</v>
+      </c>
+      <c r="N55">
+        <f>D55/(L55*wing_area)</f>
+        <v>4.1586370767179821E-5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>6.0149999999999997</v>
       </c>
@@ -6359,8 +7029,20 @@
         <f t="shared" si="1"/>
         <v>2.5899509986650089E-8</v>
       </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L56" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M56">
+        <f>B56/(L56*wing_area)</f>
+        <v>1.5986412896253004E-4</v>
+      </c>
+      <c r="N56">
+        <f>D56/(L56*wing_area)</f>
+        <v>4.1586370767179821E-5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>7.9880000000000004</v>
       </c>
@@ -6398,8 +7080,20 @@
         <f t="shared" si="1"/>
         <v>3.2451610590209183E-8</v>
       </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L57" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M57">
+        <f>B57/(L57*wing_area)</f>
+        <v>1.7894657066573096E-4</v>
+      </c>
+      <c r="N57">
+        <f>D57/(L57*wing_area)</f>
+        <v>4.7483568494699638E-5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>7.9880000000000004</v>
       </c>
@@ -6437,8 +7131,20 @@
         <f t="shared" si="1"/>
         <v>3.2451610590209183E-8</v>
       </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L58" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M58">
+        <f>B58/(L58*wing_area)</f>
+        <v>1.7894657066573096E-4</v>
+      </c>
+      <c r="N58">
+        <f>D58/(L58*wing_area)</f>
+        <v>4.7483568494699638E-5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>8.0570000000000004</v>
       </c>
@@ -6476,8 +7182,20 @@
         <f t="shared" si="1"/>
         <v>3.2572792786668466E-8</v>
       </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L59" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M59">
+        <f>B59/(L59*wing_area)</f>
+        <v>1.7928037431068491E-4</v>
+      </c>
+      <c r="N59">
+        <f>D59/(L59*wing_area)</f>
+        <v>4.500785812795783E-5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>8.0570000000000004</v>
       </c>
@@ -6515,8 +7233,20 @@
         <f t="shared" si="1"/>
         <v>3.2572792786668466E-8</v>
       </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L60" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M60">
+        <f>B60/(L60*wing_area)</f>
+        <v>1.7928037431068491E-4</v>
+      </c>
+      <c r="N60">
+        <f>D60/(L60*wing_area)</f>
+        <v>4.500785812795783E-5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>8.0570000000000004</v>
       </c>
@@ -6554,8 +7284,20 @@
         <f t="shared" si="1"/>
         <v>3.2572792786668466E-8</v>
       </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L61" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M61">
+        <f>B61/(L61*wing_area)</f>
+        <v>1.7928037431068491E-4</v>
+      </c>
+      <c r="N61">
+        <f>D61/(L61*wing_area)</f>
+        <v>4.500785812795783E-5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>9.9619999999999997</v>
       </c>
@@ -6593,8 +7335,20 @@
         <f t="shared" si="1"/>
         <v>4.0122279891789308E-8</v>
       </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L62" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M62">
+        <f>B62/(L62*wing_area)</f>
+        <v>1.9897478936296807E-4</v>
+      </c>
+      <c r="N62">
+        <f>D62/(L62*wing_area)</f>
+        <v>5.1767381938275346E-5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>9.9619999999999997</v>
       </c>
@@ -6632,8 +7386,20 @@
         <f t="shared" si="1"/>
         <v>4.0122279891789308E-8</v>
       </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L63" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M63">
+        <f>B63/(L63*wing_area)</f>
+        <v>1.9897478936296807E-4</v>
+      </c>
+      <c r="N63">
+        <f>D63/(L63*wing_area)</f>
+        <v>5.1767381938275346E-5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>9.9619999999999997</v>
       </c>
@@ -6671,8 +7437,20 @@
         <f t="shared" si="1"/>
         <v>4.0122279891789308E-8</v>
       </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L64" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M64">
+        <f>B64/(L64*wing_area)</f>
+        <v>1.9897478936296807E-4</v>
+      </c>
+      <c r="N64">
+        <f>D64/(L64*wing_area)</f>
+        <v>5.1767381938275346E-5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>10.037000000000001</v>
       </c>
@@ -6710,8 +7488,20 @@
         <f t="shared" si="1"/>
         <v>3.8150266582653179E-8</v>
       </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L65" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M65">
+        <f>B65/(L65*wing_area)</f>
+        <v>1.9402336862948445E-4</v>
+      </c>
+      <c r="N65">
+        <f>D65/(L65*wing_area)</f>
+        <v>5.0682520092175009E-5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>10.037000000000001</v>
       </c>
@@ -6749,8 +7539,20 @@
         <f t="shared" si="1"/>
         <v>3.8150266582653179E-8</v>
       </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L66" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M66">
+        <f>B66/(L66*wing_area)</f>
+        <v>1.9402336862948445E-4</v>
+      </c>
+      <c r="N66">
+        <f>D66/(L66*wing_area)</f>
+        <v>5.0682520092175009E-5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>11.99</v>
       </c>
@@ -6788,8 +7590,20 @@
         <f t="shared" ref="K67:K85" si="3">I67^2</f>
         <v>4.6420895815066445E-8</v>
       </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L67" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M67">
+        <f>B67/(L67*wing_area)</f>
+        <v>2.1402377035630873E-4</v>
+      </c>
+      <c r="N67">
+        <f>D67/(L67*wing_area)</f>
+        <v>5.524450323987901E-5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>11.99</v>
       </c>
@@ -6827,8 +7641,20 @@
         <f t="shared" si="3"/>
         <v>4.6420895815066445E-8</v>
       </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L68" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M68">
+        <f>B68/(L68*wing_area)</f>
+        <v>2.1402377035630873E-4</v>
+      </c>
+      <c r="N68">
+        <f>D68/(L68*wing_area)</f>
+        <v>5.524450323987901E-5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>12.003</v>
       </c>
@@ -6866,8 +7692,20 @@
         <f t="shared" si="3"/>
         <v>4.2987478665526836E-8</v>
       </c>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L69" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M69">
+        <f>B69/(L69*wing_area)</f>
+        <v>2.0595684893658821E-4</v>
+      </c>
+      <c r="N69">
+        <f>D69/(L69*wing_area)</f>
+        <v>5.7469860872905352E-5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>12.003</v>
       </c>
@@ -6905,8 +7743,20 @@
         <f t="shared" si="3"/>
         <v>4.2987478665526836E-8</v>
       </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L70" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M70">
+        <f>B70/(L70*wing_area)</f>
+        <v>2.0595684893658821E-4</v>
+      </c>
+      <c r="N70">
+        <f>D70/(L70*wing_area)</f>
+        <v>5.7469860872905352E-5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>12.003</v>
       </c>
@@ -6944,8 +7794,20 @@
         <f t="shared" si="3"/>
         <v>4.2987478665526836E-8</v>
       </c>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L71" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M71">
+        <f>B71/(L71*wing_area)</f>
+        <v>2.0595684893658821E-4</v>
+      </c>
+      <c r="N71">
+        <f>D71/(L71*wing_area)</f>
+        <v>5.7469860872905352E-5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>13.958</v>
       </c>
@@ -6983,8 +7845,20 @@
         <f t="shared" si="3"/>
         <v>4.304555807343669E-8</v>
       </c>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L72" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M72">
+        <f>B72/(L72*wing_area)</f>
+        <v>2.0609593378865236E-4</v>
+      </c>
+      <c r="N72">
+        <f>D72/(L72*wing_area)</f>
+        <v>6.7789956896065028E-5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>13.958</v>
       </c>
@@ -7022,8 +7896,20 @@
         <f t="shared" si="3"/>
         <v>4.304555807343669E-8</v>
       </c>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L73" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M73">
+        <f>B73/(L73*wing_area)</f>
+        <v>2.0609593378865236E-4</v>
+      </c>
+      <c r="N73">
+        <f>D73/(L73*wing_area)</f>
+        <v>6.7789956896065028E-5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>13.976000000000001</v>
       </c>
@@ -7061,8 +7947,20 @@
         <f t="shared" si="3"/>
         <v>4.304555807343669E-8</v>
       </c>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L74" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M74">
+        <f>B74/(L74*wing_area)</f>
+        <v>2.0609593378865236E-4</v>
+      </c>
+      <c r="N74">
+        <f>D74/(L74*wing_area)</f>
+        <v>6.9264256327944987E-5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>13.976000000000001</v>
       </c>
@@ -7100,8 +7998,20 @@
         <f t="shared" si="3"/>
         <v>4.304555807343669E-8</v>
       </c>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L75" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M75">
+        <f>B75/(L75*wing_area)</f>
+        <v>2.0609593378865236E-4</v>
+      </c>
+      <c r="N75">
+        <f>D75/(L75*wing_area)</f>
+        <v>6.9264256327944987E-5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>15.951000000000001</v>
       </c>
@@ -7139,8 +8049,20 @@
         <f t="shared" si="3"/>
         <v>4.5019817239917768E-8</v>
       </c>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L76" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M76">
+        <f>B76/(L76*wing_area)</f>
+        <v>2.1076918481800769E-4</v>
+      </c>
+      <c r="N76">
+        <f>D76/(L76*wing_area)</f>
+        <v>6.8262845393083138E-5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>15.951000000000001</v>
       </c>
@@ -7178,8 +8100,20 @@
         <f t="shared" si="3"/>
         <v>4.5019817239917768E-8</v>
       </c>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L77" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M77">
+        <f>B77/(L77*wing_area)</f>
+        <v>2.1076918481800769E-4</v>
+      </c>
+      <c r="N77">
+        <f>D77/(L77*wing_area)</f>
+        <v>6.8262845393083138E-5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>15.996</v>
       </c>
@@ -7217,8 +8151,20 @@
         <f t="shared" si="3"/>
         <v>4.7916973214904878E-8</v>
       </c>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L78" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M78">
+        <f>B78/(L78*wing_area)</f>
+        <v>2.1744525771708674E-4</v>
+      </c>
+      <c r="N78">
+        <f>D78/(L78*wing_area)</f>
+        <v>7.1600881842622639E-5</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>15.996</v>
       </c>
@@ -7256,8 +8202,20 @@
         <f t="shared" si="3"/>
         <v>4.7916973214904878E-8</v>
       </c>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L79" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M79">
+        <f>B79/(L79*wing_area)</f>
+        <v>2.1744525771708674E-4</v>
+      </c>
+      <c r="N79">
+        <f>D79/(L79*wing_area)</f>
+        <v>7.1600881842622639E-5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>15.996</v>
       </c>
@@ -7295,8 +8253,20 @@
         <f t="shared" si="3"/>
         <v>4.7916973214904878E-8</v>
       </c>
-    </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L80" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M80">
+        <f>B80/(L80*wing_area)</f>
+        <v>2.1744525771708674E-4</v>
+      </c>
+      <c r="N80">
+        <f>D80/(L80*wing_area)</f>
+        <v>7.1600881842622639E-5</v>
+      </c>
+    </row>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>3.3000000000000002E-2</v>
       </c>
@@ -7334,8 +8304,20 @@
         <f t="shared" si="3"/>
         <v>1.1228232802873681E-8</v>
       </c>
-    </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L81" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M81">
+        <f>B81/(L81*wing_area)</f>
+        <v>1.052594160421461E-4</v>
+      </c>
+      <c r="N81">
+        <f>D81/(L81*wing_area)</f>
+        <v>3.0904654128653364E-5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>3.3000000000000002E-2</v>
       </c>
@@ -7373,8 +8355,20 @@
         <f t="shared" si="3"/>
         <v>1.1228232802873681E-8</v>
       </c>
-    </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L82" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M82">
+        <f>B82/(L82*wing_area)</f>
+        <v>1.052594160421461E-4</v>
+      </c>
+      <c r="N82">
+        <f>D82/(L82*wing_area)</f>
+        <v>3.0904654128653364E-5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>2.1999999999999999E-2</v>
       </c>
@@ -7412,8 +8406,20 @@
         <f t="shared" si="3"/>
         <v>1.2440268845348902E-8</v>
       </c>
-    </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L83" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M83">
+        <f>B83/(L83*wing_area)</f>
+        <v>1.1079499315429915E-4</v>
+      </c>
+      <c r="N83">
+        <f>D83/(L83*wing_area)</f>
+        <v>3.1238457773607318E-5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>2.1999999999999999E-2</v>
       </c>
@@ -7451,8 +8457,20 @@
         <f t="shared" si="3"/>
         <v>1.2440268845348902E-8</v>
       </c>
-    </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L84" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M84">
+        <f>B84/(L84*wing_area)</f>
+        <v>1.1079499315429915E-4</v>
+      </c>
+      <c r="N84">
+        <f>D84/(L84*wing_area)</f>
+        <v>3.1238457773607318E-5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>2.1999999999999999E-2</v>
       </c>
@@ -7489,6 +8507,18 @@
       <c r="K85">
         <f t="shared" si="3"/>
         <v>1.2440268845348902E-8</v>
+      </c>
+      <c r="L85" s="13">
+        <f>0.5*(65*12)^2*0.002377*(1+eps_tot_t)^2</f>
+        <v>727.91914084511302</v>
+      </c>
+      <c r="M85">
+        <f>B85/(L85*wing_area)</f>
+        <v>1.1079499315429915E-4</v>
+      </c>
+      <c r="N85">
+        <f>D85/(L85*wing_area)</f>
+        <v>3.1238457773607318E-5</v>
       </c>
     </row>
   </sheetData>
@@ -12535,8 +13565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Finished Cm vs Cl graph, same work needs to be done as previous commit
</commit_message>
<xml_diff>
--- a/Formal_Lab_Tom/Wind_Tunnel_Data.xlsx
+++ b/Formal_Lab_Tom/Wind_Tunnel_Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="No wind" sheetId="1" r:id="rId1"/>
@@ -13,10 +13,11 @@
     <sheet name="CL vs Alpha " sheetId="8" r:id="rId4"/>
     <sheet name="CD vs Alpha" sheetId="9" r:id="rId5"/>
     <sheet name="Cm vs Alpha" sheetId="10" r:id="rId6"/>
-    <sheet name="Tail On 65 MPH" sheetId="2" r:id="rId7"/>
-    <sheet name="Tail OFf 65 MPH" sheetId="3" r:id="rId8"/>
-    <sheet name="No Model 65 MPH" sheetId="4" r:id="rId9"/>
-    <sheet name="Airplane Characteristics" sheetId="5" r:id="rId10"/>
+    <sheet name="Cm vs Cl" sheetId="11" r:id="rId7"/>
+    <sheet name="Tail On 65 MPH" sheetId="2" r:id="rId8"/>
+    <sheet name="Tail OFf 65 MPH" sheetId="3" r:id="rId9"/>
+    <sheet name="No Model 65 MPH" sheetId="4" r:id="rId10"/>
+    <sheet name="Airplane Characteristics" sheetId="5" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="atnt">'Airplane Characteristics'!$K$11</definedName>
@@ -54,14 +55,14 @@
     <definedName name="lamda_vt">'Airplane Characteristics'!$C$28</definedName>
     <definedName name="lamda_w">'Airplane Characteristics'!$C$6</definedName>
     <definedName name="lbar">'Airplane Characteristics'!$C$23</definedName>
-    <definedName name="NoModel65mph" localSheetId="8">'No Model 65 MPH'!$A$1:$N$75</definedName>
+    <definedName name="NoModel65mph" localSheetId="9">'No Model 65 MPH'!$A$1:$N$75</definedName>
     <definedName name="nowind" localSheetId="0">'No wind'!$A$1:$H$70</definedName>
     <definedName name="Rc_">'Airplane Characteristics'!$C$4</definedName>
     <definedName name="strut_area">'Airplane Characteristics'!$G$30</definedName>
     <definedName name="t_tail">'Airplane Characteristics'!$C$17</definedName>
     <definedName name="t_wing">'Airplane Characteristics'!$C$7</definedName>
-    <definedName name="tailoff65mph" localSheetId="7">'Tail OFf 65 MPH'!$A$1:$I$76</definedName>
-    <definedName name="tailon65mph" localSheetId="6">'Tail On 65 MPH'!$A$1:$I$85</definedName>
+    <definedName name="tailoff65mph" localSheetId="8">'Tail OFf 65 MPH'!$A$1:$I$76</definedName>
+    <definedName name="tailon65mph" localSheetId="7">'Tail On 65 MPH'!$A$1:$I$85</definedName>
     <definedName name="tamc">'Airplane Characteristics'!$C$21</definedName>
     <definedName name="tau_wing">'Airplane Characteristics'!$G$13</definedName>
     <definedName name="tau1_">'Airplane Characteristics'!$G$6</definedName>
@@ -7009,7 +7010,7 @@
                   <c:v>-3.551149095670783E-5</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>7.3220943226661456E-5</c:v>
+                  <c:v>-1.0979349573810142E-4</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>-1.0979349573810142E-4</c:v>
@@ -7024,7 +7025,7 @@
                   <c:v>-1.0979349573810142E-4</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-8.6008275760489388E-5</c:v>
+                  <c:v>-7.4716190567619567E-5</c:v>
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>-7.4716190567619567E-5</c:v>
@@ -7039,7 +7040,7 @@
                   <c:v>-7.4716190567619567E-5</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>-1.6356057492714299E-4</c:v>
+                  <c:v>-1.5749152987629575E-4</c:v>
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>-1.4707596124470006E-4</c:v>
@@ -7054,7 +7055,7 @@
                   <c:v>-1.4707596124470006E-4</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>-1.3084930971478398E-4</c:v>
+                  <c:v>-1.0024612230802088E-4</c:v>
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>-1.0024612230802088E-4</c:v>
@@ -7069,7 +7070,7 @@
                   <c:v>-1.0062058349717279E-4</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>-1.3290745936182633E-4</c:v>
+                  <c:v>2.1426619524563982E-6</c:v>
                 </c:pt>
                 <c:pt idx="36">
                   <c:v>2.1426619524563982E-6</c:v>
@@ -7084,7 +7085,7 @@
                   <c:v>2.1426619524563982E-6</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>-3.6718088121752879E-5</c:v>
+                  <c:v>-9.2387984909003429E-5</c:v>
                 </c:pt>
                 <c:pt idx="41">
                   <c:v>-9.2387984909003429E-5</c:v>
@@ -7099,7 +7100,7 @@
                   <c:v>-1.1320525323926326E-4</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>-1.597355232246209E-4</c:v>
+                  <c:v>-1.6359108657959239E-4</c:v>
                 </c:pt>
                 <c:pt idx="46">
                   <c:v>-1.6359108657959239E-4</c:v>
@@ -7114,7 +7115,7 @@
                   <c:v>-1.6893062575824001E-4</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>-2.5414134968969673E-4</c:v>
+                  <c:v>-1.8132390422587503E-4</c:v>
                 </c:pt>
                 <c:pt idx="51">
                   <c:v>-1.6947983550232945E-4</c:v>
@@ -7129,7 +7130,7 @@
                   <c:v>-1.6947983550232945E-4</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>-2.1653712493908611E-4</c:v>
+                  <c:v>-2.5034403585303777E-4</c:v>
                 </c:pt>
                 <c:pt idx="56">
                   <c:v>-2.5034403585303777E-4</c:v>
@@ -7144,7 +7145,7 @@
                   <c:v>-2.3096913654765925E-4</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>-2.5042724945062704E-4</c:v>
+                  <c:v>-1.8752262379963234E-4</c:v>
                 </c:pt>
                 <c:pt idx="61">
                   <c:v>-1.8752262379963234E-4</c:v>
@@ -7159,46 +7160,46 @@
                   <c:v>-1.9641260980875726E-4</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>-1.416559822550494E-4</c:v>
+                  <c:v>-1.7293042601569962E-4</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>-1.416559822550494E-4</c:v>
+                  <c:v>-1.7293042601569962E-4</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>-1.5017150707502248E-4</c:v>
+                  <c:v>-1.814459508356727E-4</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>-1.5017150707502248E-4</c:v>
+                  <c:v>-1.814459508356727E-4</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>-1.5017150707502248E-4</c:v>
+                  <c:v>-1.814459508356727E-4</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>-2.1382158787108818E-4</c:v>
+                  <c:v>-2.0609104465504094E-4</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>-2.1382158787108818E-4</c:v>
+                  <c:v>-2.0609104465504094E-4</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>-2.164150783292885E-4</c:v>
+                  <c:v>-2.0868453511324126E-4</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>-2.164150783292885E-4</c:v>
+                  <c:v>-2.0868453511324126E-4</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>-2.2839783638214955E-4</c:v>
+                  <c:v>-2.2710525183292887E-4</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>-2.2839783638214955E-4</c:v>
+                  <c:v>-2.2710525183292887E-4</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>-2.5810509072153441E-4</c:v>
+                  <c:v>-2.5681250617231373E-4</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>-2.5810509072153441E-4</c:v>
+                  <c:v>-2.5681250617231373E-4</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>-2.5810509072153441E-4</c:v>
+                  <c:v>-2.5681250617231373E-4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8055,49 +8056,49 @@
                   <c:v>-7.1938936748076231E-5</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>-3.0413271211069196E-5</c:v>
+                  <c:v>-6.168771497171941E-5</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>-3.0413271211069196E-5</c:v>
+                  <c:v>-6.168771497171941E-5</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>-3.0413271211069196E-5</c:v>
+                  <c:v>-6.168771497171941E-5</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>-2.9553397369312944E-5</c:v>
+                  <c:v>-6.0827841129963158E-5</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>-2.9553397369312944E-5</c:v>
+                  <c:v>-6.0827841129963158E-5</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>-5.9307806080665087E-5</c:v>
+                  <c:v>-5.1577262864617847E-5</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>-5.9307806080665087E-5</c:v>
+                  <c:v>-5.1577262864617847E-5</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>-5.9307806080665087E-5</c:v>
+                  <c:v>-5.1577262864617847E-5</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>-6.6561258003866889E-5</c:v>
+                  <c:v>-5.8830714787819649E-5</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>-6.6561258003866889E-5</c:v>
+                  <c:v>-5.8830714787819649E-5</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>-1.1130243564105429E-4</c:v>
+                  <c:v>-1.1000985109183362E-4</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>-1.1130243564105429E-4</c:v>
+                  <c:v>-1.1000985109183362E-4</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>-1.1130243564105429E-4</c:v>
+                  <c:v>-1.1000985109183362E-4</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>-1.1130243564105429E-4</c:v>
+                  <c:v>-1.1000985109183362E-4</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>-8.3800341637786289E-5</c:v>
+                  <c:v>-8.2507757088565615E-5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8203,6 +8204,2065 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0">
+                <a:effectLst/>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t>CM vs CL both With and Without Tail with Freestream Airspeed of 65 fps, Static Temp 70 ⁰F, and Standard Atmospheric Pressure</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:effectLst/>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Non-Corrected Tail</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Tail On 65 MPH'!$J$2:$J$80</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="79"/>
+                <c:pt idx="0">
+                  <c:v>1.121800221751813E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.121800221751813E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.121800221751813E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.121800221751813E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.1192799516580121E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.1402822024396861E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.1402822024396861E-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.1402822024396861E-4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.1402822024396861E-4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.1904075743052814E-4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.5154197541504263E-5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.061313739500592E-4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.061313739500592E-4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.061313739500592E-4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.061313739500592E-4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.4166589899446194E-5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.4166589899446194E-5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.4166589899446194E-5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.4166589899446194E-5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.4166589899446194E-5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5.3065686975029598E-5</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5.3065686975029598E-5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5.3065686975029598E-5</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>5.3065686975029598E-5</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>5.3065686975029598E-5</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>6.2642713331472938E-5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>6.9391436582650837E-5</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>6.9391436582650837E-5</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>6.9391436582650837E-5</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>6.9391436582650837E-5</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>8.7789408267397234E-5</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>8.7789408267397234E-5</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>9.378205049043489E-5</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>9.378205049043489E-5</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>9.378205049043489E-5</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>9.932664469679682E-5</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>9.932664469679682E-5</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>9.932664469679682E-5</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>9.932664469679682E-5</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>9.932664469679682E-5</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1.2676958571818415E-4</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1.2676958571818415E-4</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1.232132045858207E-4</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1.232132045858207E-4</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1.232132045858207E-4</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1.4838790252278726E-4</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1.4838790252278726E-4</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1.5412851773644479E-4</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1.5412851773644479E-4</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1.5412851773644479E-4</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1.7031425233885489E-4</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>1.6093324698970716E-4</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1.6093324698970716E-4</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1.6093324698970716E-4</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1.6093324698970716E-4</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>1.801433057046783E-4</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>1.801433057046783E-4</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>1.8047934171718508E-4</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>1.8047934171718508E-4</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1.8047934171718508E-4</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>2.0030546645508532E-4</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>2.0030546645508532E-4</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>2.0030546645508532E-4</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>1.9532093226956801E-4</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>1.9532093226956801E-4</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>2.1545509001893282E-4</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>2.1545509001893282E-4</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>2.0733421971668554E-4</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>2.0733421971668554E-4</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>2.0733421971668554E-4</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>2.074742347218967E-4</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>2.074742347218967E-4</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>2.074742347218967E-4</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>2.074742347218967E-4</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>2.1217873889699167E-4</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>2.1217873889699167E-4</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>2.1889945914712735E-4</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>2.1889945914712735E-4</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>2.1889945914712735E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Tail On 65 MPH'!$R$2:$R$80</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="79"/>
+                <c:pt idx="0">
+                  <c:v>-1.2429762579791874E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-1.2429762579791874E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-1.2429762579791874E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-1.2429762579791874E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-1.4916462254419181E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-1.5261798684414833E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-1.5261798684414833E-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-1.5261798684414833E-4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-1.5261798684414833E-4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-1.475419573912002E-4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-1.5217418099033867E-4</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-1.7494696886394736E-4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-1.7494696886394736E-4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-1.7494696886394736E-4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-1.7494696886394736E-4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-6.6214534680578079E-5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-6.6214534680578079E-5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-6.6214534680578079E-5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-6.6214534680578079E-5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-6.6214534680578079E-5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-4.2429314702966049E-5</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-4.2429314702966049E-5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-4.2429314702966049E-5</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-4.2429314702966049E-5</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-4.2429314702966049E-5</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-1.3127369906248946E-4</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-1.2085813043089376E-4</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-1.2085813043089376E-4</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-1.2085813043089376E-4</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-1.2085813043089376E-4</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-1.0463147890097768E-4</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-1.0463147890097768E-4</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-1.0500594009012959E-4</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>-1.0500594009012959E-4</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>-1.0500594009012959E-4</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>-1.3729281595478314E-4</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>-1.3729281595478314E-4</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>-1.3729281595478314E-4</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>-1.3729281595478314E-4</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>-1.3729281595478314E-4</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>-1.7615356602899241E-4</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>-1.7615356602899241E-4</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>-1.9697083435925224E-4</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>-1.9697083435925224E-4</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>-1.9697083435925224E-4</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>-2.4350110434460988E-4</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>-2.4350110434460988E-4</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>-2.4884064352325748E-4</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>-2.4884064352325748E-4</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>-2.4884064352325748E-4</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>-3.340513674547142E-4</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>-3.2220729873116863E-4</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>-3.2220729873116863E-4</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>-3.2220729873116863E-4</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>-3.2220729873116863E-4</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>-3.6926458816792529E-4</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>-3.6926458816792529E-4</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>-3.498896888625468E-4</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>-3.498896888625468E-4</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>-3.498896888625468E-4</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>-3.6934780176551462E-4</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>-3.6934780176551462E-4</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>-3.6934780176551462E-4</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>-3.7823778777463954E-4</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>-3.7823778777463954E-4</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>-4.2017744095965338E-4</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>-4.2017744095965338E-4</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>-4.2869296577962646E-4</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>-4.2869296577962646E-4</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>-4.2869296577962646E-4</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>-4.8461250335964491E-4</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>-4.8461250335964491E-4</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>-4.8720599381784523E-4</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>-4.8720599381784523E-4</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>-4.9204625141095694E-4</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>-4.9204625141095694E-4</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>-5.217535057503418E-4</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>-5.217535057503418E-4</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>-5.217535057503418E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Corrected Tail</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Tail On 65 MPH'!$N$2:$N$80</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="79"/>
+                <c:pt idx="0">
+                  <c:v>1.1143478347379423E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.1143478347379423E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1143478347379423E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.1143478347379423E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.1118443074007875E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.1327070352104096E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.1327070352104096E-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.1327070352104096E-4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.1327070352104096E-4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.1824994122493741E-4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.4522065462794E-5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.0542631786462309E-4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.0542631786462309E-4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.0542631786462309E-4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.0542631786462309E-4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.4006045466271695E-5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.4006045466271695E-5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.4006045466271695E-5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.4006045466271695E-5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.4006045466271695E-5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5.2713158932311547E-5</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5.2713158932311547E-5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5.2713158932311547E-5</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>5.2713158932311547E-5</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>5.2713158932311547E-5</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>6.2226562813499171E-5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>6.8930452682991033E-5</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>6.8930452682991033E-5</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>6.8930452682991033E-5</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>6.8930452682991033E-5</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>8.7206202244219884E-5</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>8.7206202244219884E-5</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>9.3159033912565363E-5</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>9.3159033912565363E-5</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>9.3159033912565363E-5</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>9.8666794054305578E-5</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>9.8666794054305578E-5</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>9.8666794054305578E-5</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>9.8666794054305578E-5</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>9.8666794054305578E-5</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1.259274250588783E-4</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1.259274250588783E-4</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1.2239466981644898E-4</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1.2239466981644898E-4</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1.2239466981644898E-4</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1.4740212621758254E-4</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1.4740212621758254E-4</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1.5310460515221251E-4</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1.5310460515221251E-4</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1.5310460515221251E-4</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1.6918281405082787E-4</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>1.5986412896253004E-4</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1.5986412896253004E-4</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1.5986412896253004E-4</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1.5986412896253004E-4</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>1.7894657066573096E-4</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>1.7894657066573096E-4</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>1.7928037431068491E-4</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>1.7928037431068491E-4</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1.7928037431068491E-4</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>1.9897478936296807E-4</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>1.9897478936296807E-4</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>1.9897478936296807E-4</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>1.9402336862948445E-4</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>1.9402336862948445E-4</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>2.1402377035630873E-4</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>2.1402377035630873E-4</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>2.0595684893658821E-4</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>2.0595684893658821E-4</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>2.0595684893658821E-4</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>2.0609593378865236E-4</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>2.0609593378865236E-4</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>2.0609593378865236E-4</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>2.0609593378865236E-4</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>2.1076918481800769E-4</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>2.1076918481800769E-4</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>2.1744525771708674E-4</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>2.1744525771708674E-4</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>2.1744525771708674E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Tail On 65 MPH'!$S$2:$S$80</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="79"/>
+                <c:pt idx="0">
+                  <c:v>1.5137852109320794E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5137852109320794E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5137852109320794E-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5137852109320794E-5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-9.7291446369522779E-6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-1.3182508936908794E-5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-1.3182508936908794E-5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-1.3182508936908794E-5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-1.3182508936908794E-5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-8.1064794839606671E-6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-1.2738703083099132E-5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-3.551149095670783E-5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-3.551149095670783E-5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-3.551149095670783E-5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-3.551149095670783E-5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-1.0979349573810142E-4</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-1.0979349573810142E-4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-1.0979349573810142E-4</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-1.0979349573810142E-4</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-1.0979349573810142E-4</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-7.4716190567619567E-5</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-7.4716190567619567E-5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-7.4716190567619567E-5</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-7.4716190567619567E-5</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-7.4716190567619567E-5</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-1.5749152987629575E-4</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-1.4707596124470006E-4</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-1.4707596124470006E-4</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-1.4707596124470006E-4</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-1.4707596124470006E-4</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-1.0024612230802088E-4</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-1.0024612230802088E-4</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-1.0062058349717279E-4</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>-1.0062058349717279E-4</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>-1.0062058349717279E-4</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2.1426619524563982E-6</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2.1426619524563982E-6</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2.1426619524563982E-6</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2.1426619524563982E-6</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2.1426619524563982E-6</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>-9.2387984909003429E-5</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>-9.2387984909003429E-5</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>-1.1320525323926326E-4</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>-1.1320525323926326E-4</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>-1.1320525323926326E-4</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>-1.6359108657959239E-4</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>-1.6359108657959239E-4</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>-1.6893062575824001E-4</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>-1.6893062575824001E-4</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>-1.6893062575824001E-4</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>-1.8132390422587503E-4</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>-1.6947983550232945E-4</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>-1.6947983550232945E-4</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>-1.6947983550232945E-4</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>-1.6947983550232945E-4</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>-2.5034403585303777E-4</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>-2.5034403585303777E-4</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>-2.3096913654765925E-4</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>-2.3096913654765925E-4</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>-2.3096913654765925E-4</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>-1.8752262379963234E-4</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>-1.8752262379963234E-4</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>-1.8752262379963234E-4</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>-1.9641260980875726E-4</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>-1.9641260980875726E-4</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>-1.7293042601569962E-4</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>-1.7293042601569962E-4</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>-1.814459508356727E-4</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>-1.814459508356727E-4</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>-1.814459508356727E-4</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>-2.0609104465504094E-4</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>-2.0609104465504094E-4</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>-2.0868453511324126E-4</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>-2.0868453511324126E-4</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>-2.2710525183292887E-4</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>-2.2710525183292887E-4</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>-2.5681250617231373E-4</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>-2.5681250617231373E-4</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>-2.5681250617231373E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Non-Corrected No Tail</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Tail OFf 65 MPH'!$J$2:$J$71</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="70"/>
+                <c:pt idx="0">
+                  <c:v>1.0618737995214365E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0618737995214365E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0159488778121762E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0159488778121762E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0159488778121762E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.9966139743111398E-5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.9966139743111398E-5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.6269743605536778E-5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.6269743605536778E-5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.6269743605536778E-5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.9316213463293693E-5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.9316213463293693E-5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.9316213463293693E-5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.3379577242340516E-5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.3379577242340516E-5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.4297819020887804E-5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5.4297819020887804E-5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5.4297819020887804E-5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5.9254350205362863E-5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5.9254350205362863E-5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>8.1292712025599431E-5</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>8.1292712025599431E-5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>8.1292712025599431E-5</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>8.3504949107935763E-5</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>8.3504949107935763E-5</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>9.876658467595218E-5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>9.876658467595218E-5</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>9.876658467595218E-5</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>9.876658467595218E-5</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>9.5350218548799866E-5</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.1430825025439092E-4</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1.0778355101155087E-4</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1.0778355101155087E-4</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1.0778355101155087E-4</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1.0778355101155087E-4</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1.3553452504440276E-4</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1.3553452504440276E-4</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1.3553452504440276E-4</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1.4141515526327146E-4</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1.4141515526327146E-4</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1.6258542405119886E-4</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1.6258542405119886E-4</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1.6258542405119886E-4</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1.5522063477709183E-4</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1.5522063477709183E-4</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1.7233046841389559E-4</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1.7233046841389559E-4</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1.7233046841389559E-4</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1.7731500259941286E-4</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1.7731500259941286E-4</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1.9011237407571288E-4</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>1.9011237407571288E-4</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1.9011237407571288E-4</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1.9011237407571288E-4</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1.9358474620494965E-4</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>1.9232461115804923E-4</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>1.9232461115804923E-4</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>1.9232461115804923E-4</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>1.9431282423204769E-4</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1.9431282423204769E-4</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>1.9879330439880481E-4</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>1.9879330439880481E-4</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>1.9879330439880481E-4</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>1.9798121736858007E-4</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>1.9798121736858007E-4</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>1.986252863925514E-4</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>1.986252863925514E-4</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>1.986252863925514E-4</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>1.986252863925514E-4</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>2.0013744844883194E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Tail OFf 65 MPH'!$R$2:$R$71</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="70"/>
+                <c:pt idx="0">
+                  <c:v>-1.1388205716632299E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-1.1388205716632299E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-1.032307166748909E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-1.032307166748909E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-1.032307166748909E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-1.5109240422167756E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-1.5109240422167756E-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-1.3324308753876989E-4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-1.3324308753876989E-4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-1.3324308753876989E-4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-8.4410574686774568E-5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-8.4410574686774568E-5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-8.4410574686774568E-5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-8.3106894991208667E-5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-8.3106894991208667E-5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-9.2385211122417079E-5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-9.2385211122417079E-5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-9.2385211122417079E-5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-9.3466987891078162E-5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-9.3466987891078162E-5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-1.0776585774350847E-4</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-1.0776585774350847E-4</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-1.0776585774350847E-4</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-1.0597676539533824E-4</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-1.0597676539533824E-4</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-1.3873518497966455E-4</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-1.3873518497966455E-4</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-1.3873518497966455E-4</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-1.3873518497966455E-4</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-1.330350535447966E-4</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-1.5530855983286943E-4</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-1.4651565635426535E-4</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-1.4651565635426535E-4</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>-1.4651565635426535E-4</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>-1.4651565635426535E-4</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>-1.9459924682795683E-4</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>-1.9459924682795683E-4</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>-1.9459924682795683E-4</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>-1.8647205213006724E-4</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>-1.8647205213006724E-4</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>-1.8652752786179344E-4</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>-1.8652752786179344E-4</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>-1.8652752786179344E-4</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>-1.9409996524242097E-4</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>-1.9409996524242097E-4</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>-2.2855039464439664E-4</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>-2.2855039464439664E-4</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>-2.2855039464439664E-4</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>-2.3927107980048647E-4</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>-2.3927107980048647E-4</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>-2.6584395529734051E-4</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>-2.6584395529734051E-4</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>-2.6584395529734051E-4</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>-2.6584395529734051E-4</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>-2.5376411471395851E-4</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>-3.0893472991567317E-4</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>-3.0893472991567317E-4</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>-3.0893472991567317E-4</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>-3.0807485607391692E-4</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>-3.0807485607391692E-4</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>-3.3009872156922182E-4</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>-3.3009872156922182E-4</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>-3.3009872156922182E-4</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>-3.3735217349242363E-4</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>-3.3735217349242363E-4</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>-3.7495085066986168E-4</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>-3.7495085066986168E-4</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>-3.7495085066986168E-4</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>-3.7495085066986168E-4</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>-3.4744875666659368E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Corrected No Tail</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Tail OFf 65 MPH'!$J$2:$J$71</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="70"/>
+                <c:pt idx="0">
+                  <c:v>1.0618737995214365E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0618737995214365E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0159488778121762E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0159488778121762E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0159488778121762E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.9966139743111398E-5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.9966139743111398E-5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.6269743605536778E-5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.6269743605536778E-5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.6269743605536778E-5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.9316213463293693E-5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.9316213463293693E-5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.9316213463293693E-5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.3379577242340516E-5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.3379577242340516E-5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.4297819020887804E-5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5.4297819020887804E-5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5.4297819020887804E-5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5.9254350205362863E-5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5.9254350205362863E-5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>8.1292712025599431E-5</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>8.1292712025599431E-5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>8.1292712025599431E-5</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>8.3504949107935763E-5</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>8.3504949107935763E-5</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>9.876658467595218E-5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>9.876658467595218E-5</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>9.876658467595218E-5</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>9.876658467595218E-5</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>9.5350218548799866E-5</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.1430825025439092E-4</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1.0778355101155087E-4</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1.0778355101155087E-4</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1.0778355101155087E-4</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1.0778355101155087E-4</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1.3553452504440276E-4</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1.3553452504440276E-4</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1.3553452504440276E-4</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1.4141515526327146E-4</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1.4141515526327146E-4</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1.6258542405119886E-4</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1.6258542405119886E-4</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1.6258542405119886E-4</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1.5522063477709183E-4</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1.5522063477709183E-4</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1.7233046841389559E-4</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1.7233046841389559E-4</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1.7233046841389559E-4</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1.7731500259941286E-4</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1.7731500259941286E-4</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1.9011237407571288E-4</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>1.9011237407571288E-4</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1.9011237407571288E-4</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1.9011237407571288E-4</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1.9358474620494965E-4</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>1.9232461115804923E-4</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>1.9232461115804923E-4</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>1.9232461115804923E-4</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>1.9431282423204769E-4</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1.9431282423204769E-4</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>1.9879330439880481E-4</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>1.9879330439880481E-4</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>1.9879330439880481E-4</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>1.9798121736858007E-4</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>1.9798121736858007E-4</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>1.986252863925514E-4</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>1.986252863925514E-4</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>1.986252863925514E-4</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>1.986252863925514E-4</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>2.0013744844883194E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Tail OFf 65 MPH'!$S$2:$S$71</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="70"/>
+                <c:pt idx="0">
+                  <c:v>2.5553420740916544E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5553420740916544E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.6204761232348635E-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.6204761232348635E-5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.6204761232348635E-5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-1.946713652792009E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-1.946713652792009E-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-1.7682204859629323E-4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-1.7682204859629323E-4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-1.7682204859629323E-4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-1.1669745055142809E-4</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-1.1669745055142809E-4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-1.1669745055142809E-4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-1.1539377085586219E-4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-1.1539377085586219E-4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-1.1860304193622336E-4</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-1.1860304193622336E-4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-1.1860304193622336E-4</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-1.1968481870488445E-4</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-1.1968481870488445E-4</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-1.0338050115055167E-4</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-1.0338050115055167E-4</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-1.0338050115055167E-4</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-1.0159140880238144E-4</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-1.0159140880238144E-4</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>7.0029292757498138E-7</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>7.0029292757498138E-7</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>7.0029292757498138E-7</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>7.0029292757498138E-7</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>6.4004243624429379E-6</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-7.1542978712880448E-5</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-6.2750075234276363E-5</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-6.2750075234276363E-5</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>-6.2750075234276363E-5</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>-6.2750075234276363E-5</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>-1.1468922906293935E-4</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>-1.1468922906293935E-4</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>-1.1468922906293935E-4</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>-1.0656203436504976E-4</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>-1.0656203436504976E-4</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>-3.380006463295427E-5</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>-3.380006463295427E-5</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>-3.380006463295427E-5</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>-4.1372502013581797E-5</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>-4.1372502013581797E-5</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>-1.096298423295091E-4</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>-1.096298423295091E-4</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>-1.096298423295091E-4</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>-1.2035052748559893E-4</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>-1.2035052748559893E-4</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>-8.4018777331458229E-5</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>-8.4018777331458229E-5</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>-8.4018777331458229E-5</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>-8.4018777331458229E-5</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>-7.1938936748076231E-5</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>-6.168771497171941E-5</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>-6.168771497171941E-5</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>-6.168771497171941E-5</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>-6.0827841129963158E-5</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>-6.0827841129963158E-5</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>-5.1577262864617847E-5</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>-5.1577262864617847E-5</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>-5.1577262864617847E-5</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>-5.8830714787819649E-5</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>-5.8830714787819649E-5</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>-1.1000985109183362E-4</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>-1.1000985109183362E-4</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>-1.1000985109183362E-4</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>-1.1000985109183362E-4</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>-8.2507757088565615E-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="180172288"/>
+        <c:axId val="180173824"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="180172288"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US">
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>CL</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="180173824"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="180173824"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US">
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>CM</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="180172288"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
@@ -8248,6 +10308,17 @@
 </file>
 
 <file path=xl/chartsheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="115" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
@@ -8367,6 +10438,33 @@
 </file>
 
 <file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8663609" cy="6286500"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
@@ -10611,8 +12709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S85"/>
   <sheetViews>
-    <sheetView topLeftCell="C2" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2:R80"/>
+    <sheetView topLeftCell="F44" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2:R81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11825,8 +13923,8 @@
         <v>-6.6214534680578079E-5</v>
       </c>
       <c r="S17">
-        <f>R17-'No Model 65 MPH'!$Q$12</f>
-        <v>7.3220943226661456E-5</v>
+        <f>R17-'No Model 65 MPH'!$Q$8</f>
+        <v>-1.0979349573810142E-4</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
@@ -12180,8 +14278,8 @@
         <v>-4.2429314702966049E-5</v>
       </c>
       <c r="S22">
-        <f>R22-'No Model 65 MPH'!$Q$8</f>
-        <v>-8.6008275760489388E-5</v>
+        <f>R22-'No Model 65 MPH'!$Q$9</f>
+        <v>-7.4716190567619567E-5</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
@@ -12535,8 +14633,8 @@
         <v>-1.3127369906248946E-4</v>
       </c>
       <c r="S27">
-        <f>R27-'No Model 65 MPH'!$Q$9</f>
-        <v>-1.6356057492714299E-4</v>
+        <f>R27-'No Model 65 MPH'!$Q$10</f>
+        <v>-1.5749152987629575E-4</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
@@ -12890,8 +14988,8 @@
         <v>-1.0463147890097768E-4</v>
       </c>
       <c r="S32">
-        <f>R32-'No Model 65 MPH'!$Q$10</f>
-        <v>-1.3084930971478398E-4</v>
+        <f>R32-'No Model 65 MPH'!$Q$11</f>
+        <v>-1.0024612230802088E-4</v>
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
@@ -13245,8 +15343,8 @@
         <v>-1.3729281595478314E-4</v>
       </c>
       <c r="S37">
-        <f>R37-'No Model 65 MPH'!$Q$11</f>
-        <v>-1.3290745936182633E-4</v>
+        <f>R37-'No Model 65 MPH'!$Q$12</f>
+        <v>2.1426619524563982E-6</v>
       </c>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.25">
@@ -13600,8 +15698,8 @@
         <v>-1.7615356602899241E-4</v>
       </c>
       <c r="S42">
-        <f>R42-'No Model 65 MPH'!$Q$12</f>
-        <v>-3.6718088121752879E-5</v>
+        <f>R42-'No Model 65 MPH'!$Q$13</f>
+        <v>-9.2387984909003429E-5</v>
       </c>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.25">
@@ -13955,8 +16053,8 @@
         <v>-2.4350110434460988E-4</v>
       </c>
       <c r="S47">
-        <f>R47-'No Model 65 MPH'!$Q$13</f>
-        <v>-1.597355232246209E-4</v>
+        <f>R47-'No Model 65 MPH'!$Q$14</f>
+        <v>-1.6359108657959239E-4</v>
       </c>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.25">
@@ -14310,8 +16408,8 @@
         <v>-3.340513674547142E-4</v>
       </c>
       <c r="S52">
-        <f>R52-'No Model 65 MPH'!$Q$14</f>
-        <v>-2.5414134968969673E-4</v>
+        <f>R52-'No Model 65 MPH'!$Q$15</f>
+        <v>-1.8132390422587503E-4</v>
       </c>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.25">
@@ -14665,8 +16763,8 @@
         <v>-3.6926458816792529E-4</v>
       </c>
       <c r="S57">
-        <f>R57-'No Model 65 MPH'!$Q$15</f>
-        <v>-2.1653712493908611E-4</v>
+        <f>R57-'No Model 65 MPH'!$Q$16</f>
+        <v>-2.5034403585303777E-4</v>
       </c>
     </row>
     <row r="58" spans="1:19" x14ac:dyDescent="0.25">
@@ -15020,8 +17118,8 @@
         <v>-3.6934780176551462E-4</v>
       </c>
       <c r="S62">
-        <f>R62-'No Model 65 MPH'!$Q$16</f>
-        <v>-2.5042724945062704E-4</v>
+        <f>R62-'No Model 65 MPH'!$Q$17</f>
+        <v>-1.8752262379963234E-4</v>
       </c>
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.25">
@@ -15376,7 +17474,7 @@
       </c>
       <c r="S67">
         <f>R67-'No Model 65 MPH'!$Q$18</f>
-        <v>-1.416559822550494E-4</v>
+        <v>-1.7293042601569962E-4</v>
       </c>
     </row>
     <row r="68" spans="1:19" x14ac:dyDescent="0.25">
@@ -15447,7 +17545,7 @@
       </c>
       <c r="S68">
         <f>R68-'No Model 65 MPH'!$Q$18</f>
-        <v>-1.416559822550494E-4</v>
+        <v>-1.7293042601569962E-4</v>
       </c>
     </row>
     <row r="69" spans="1:19" x14ac:dyDescent="0.25">
@@ -15518,7 +17616,7 @@
       </c>
       <c r="S69">
         <f>R69-'No Model 65 MPH'!$Q$18</f>
-        <v>-1.5017150707502248E-4</v>
+        <v>-1.814459508356727E-4</v>
       </c>
     </row>
     <row r="70" spans="1:19" x14ac:dyDescent="0.25">
@@ -15589,7 +17687,7 @@
       </c>
       <c r="S70">
         <f>R70-'No Model 65 MPH'!$Q$18</f>
-        <v>-1.5017150707502248E-4</v>
+        <v>-1.814459508356727E-4</v>
       </c>
     </row>
     <row r="71" spans="1:19" x14ac:dyDescent="0.25">
@@ -15660,7 +17758,7 @@
       </c>
       <c r="S71">
         <f>R71-'No Model 65 MPH'!$Q$18</f>
-        <v>-1.5017150707502248E-4</v>
+        <v>-1.814459508356727E-4</v>
       </c>
     </row>
     <row r="72" spans="1:19" x14ac:dyDescent="0.25">
@@ -15731,7 +17829,7 @@
       </c>
       <c r="S72">
         <f>R72-'No Model 65 MPH'!$Q$19</f>
-        <v>-2.1382158787108818E-4</v>
+        <v>-2.0609104465504094E-4</v>
       </c>
     </row>
     <row r="73" spans="1:19" x14ac:dyDescent="0.25">
@@ -15802,7 +17900,7 @@
       </c>
       <c r="S73">
         <f>R73-'No Model 65 MPH'!$Q$19</f>
-        <v>-2.1382158787108818E-4</v>
+        <v>-2.0609104465504094E-4</v>
       </c>
     </row>
     <row r="74" spans="1:19" x14ac:dyDescent="0.25">
@@ -15873,7 +17971,7 @@
       </c>
       <c r="S74">
         <f>R74-'No Model 65 MPH'!$Q$19</f>
-        <v>-2.164150783292885E-4</v>
+        <v>-2.0868453511324126E-4</v>
       </c>
     </row>
     <row r="75" spans="1:19" x14ac:dyDescent="0.25">
@@ -15944,7 +18042,7 @@
       </c>
       <c r="S75">
         <f>R75-'No Model 65 MPH'!$Q$19</f>
-        <v>-2.164150783292885E-4</v>
+        <v>-2.0868453511324126E-4</v>
       </c>
     </row>
     <row r="76" spans="1:19" x14ac:dyDescent="0.25">
@@ -16015,7 +18113,7 @@
       </c>
       <c r="S76">
         <f>R76-'No Model 65 MPH'!$Q$20</f>
-        <v>-2.2839783638214955E-4</v>
+        <v>-2.2710525183292887E-4</v>
       </c>
     </row>
     <row r="77" spans="1:19" x14ac:dyDescent="0.25">
@@ -16086,7 +18184,7 @@
       </c>
       <c r="S77">
         <f>R77-'No Model 65 MPH'!$Q$20</f>
-        <v>-2.2839783638214955E-4</v>
+        <v>-2.2710525183292887E-4</v>
       </c>
     </row>
     <row r="78" spans="1:19" x14ac:dyDescent="0.25">
@@ -16157,7 +18255,7 @@
       </c>
       <c r="S78">
         <f>R78-'No Model 65 MPH'!$Q$20</f>
-        <v>-2.5810509072153441E-4</v>
+        <v>-2.5681250617231373E-4</v>
       </c>
     </row>
     <row r="79" spans="1:19" x14ac:dyDescent="0.25">
@@ -16228,7 +18326,7 @@
       </c>
       <c r="S79">
         <f>R79-'No Model 65 MPH'!$Q$20</f>
-        <v>-2.5810509072153441E-4</v>
+        <v>-2.5681250617231373E-4</v>
       </c>
     </row>
     <row r="80" spans="1:19" x14ac:dyDescent="0.25">
@@ -16299,7 +18397,7 @@
       </c>
       <c r="S80">
         <f>R80-'No Model 65 MPH'!$Q$20</f>
-        <v>-2.5810509072153441E-4</v>
+        <v>-2.5681250617231373E-4</v>
       </c>
     </row>
     <row r="81" spans="1:19" x14ac:dyDescent="0.25">
@@ -16666,8 +18764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S85"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="S73" sqref="S73"/>
+    <sheetView topLeftCell="B39" workbookViewId="0">
+      <selection activeCell="S77" sqref="S77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20721,7 +22819,7 @@
       </c>
       <c r="S57">
         <f>R57-'No Model 65 MPH'!$Q$18</f>
-        <v>-3.0413271211069196E-5</v>
+        <v>-6.168771497171941E-5</v>
       </c>
     </row>
     <row r="58" spans="1:19" x14ac:dyDescent="0.25">
@@ -20792,7 +22890,7 @@
       </c>
       <c r="S58">
         <f>R58-'No Model 65 MPH'!$Q$18</f>
-        <v>-3.0413271211069196E-5</v>
+        <v>-6.168771497171941E-5</v>
       </c>
     </row>
     <row r="59" spans="1:19" x14ac:dyDescent="0.25">
@@ -20863,7 +22961,7 @@
       </c>
       <c r="S59">
         <f>R59-'No Model 65 MPH'!$Q$18</f>
-        <v>-3.0413271211069196E-5</v>
+        <v>-6.168771497171941E-5</v>
       </c>
     </row>
     <row r="60" spans="1:19" x14ac:dyDescent="0.25">
@@ -20934,7 +23032,7 @@
       </c>
       <c r="S60">
         <f>R60-'No Model 65 MPH'!$Q$18</f>
-        <v>-2.9553397369312944E-5</v>
+        <v>-6.0827841129963158E-5</v>
       </c>
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.25">
@@ -21005,7 +23103,7 @@
       </c>
       <c r="S61">
         <f>R61-'No Model 65 MPH'!$Q$18</f>
-        <v>-2.9553397369312944E-5</v>
+        <v>-6.0827841129963158E-5</v>
       </c>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.25">
@@ -21076,7 +23174,7 @@
       </c>
       <c r="S62">
         <f>R62-'No Model 65 MPH'!$Q$19</f>
-        <v>-5.9307806080665087E-5</v>
+        <v>-5.1577262864617847E-5</v>
       </c>
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.25">
@@ -21147,7 +23245,7 @@
       </c>
       <c r="S63">
         <f>R63-'No Model 65 MPH'!$Q$19</f>
-        <v>-5.9307806080665087E-5</v>
+        <v>-5.1577262864617847E-5</v>
       </c>
     </row>
     <row r="64" spans="1:19" x14ac:dyDescent="0.25">
@@ -21218,7 +23316,7 @@
       </c>
       <c r="S64">
         <f>R64-'No Model 65 MPH'!$Q$19</f>
-        <v>-5.9307806080665087E-5</v>
+        <v>-5.1577262864617847E-5</v>
       </c>
     </row>
     <row r="65" spans="1:19" x14ac:dyDescent="0.25">
@@ -21289,7 +23387,7 @@
       </c>
       <c r="S65">
         <f>R65-'No Model 65 MPH'!$Q$19</f>
-        <v>-6.6561258003866889E-5</v>
+        <v>-5.8830714787819649E-5</v>
       </c>
     </row>
     <row r="66" spans="1:19" x14ac:dyDescent="0.25">
@@ -21360,7 +23458,7 @@
       </c>
       <c r="S66">
         <f>R66-'No Model 65 MPH'!$Q$19</f>
-        <v>-6.6561258003866889E-5</v>
+        <v>-5.8830714787819649E-5</v>
       </c>
     </row>
     <row r="67" spans="1:19" x14ac:dyDescent="0.25">
@@ -21431,7 +23529,7 @@
       </c>
       <c r="S67">
         <f>R67-'No Model 65 MPH'!$Q$20</f>
-        <v>-1.1130243564105429E-4</v>
+        <v>-1.1000985109183362E-4</v>
       </c>
     </row>
     <row r="68" spans="1:19" x14ac:dyDescent="0.25">
@@ -21502,7 +23600,7 @@
       </c>
       <c r="S68">
         <f>R68-'No Model 65 MPH'!$Q$20</f>
-        <v>-1.1130243564105429E-4</v>
+        <v>-1.1000985109183362E-4</v>
       </c>
     </row>
     <row r="69" spans="1:19" x14ac:dyDescent="0.25">
@@ -21573,7 +23671,7 @@
       </c>
       <c r="S69">
         <f>R69-'No Model 65 MPH'!$Q$20</f>
-        <v>-1.1130243564105429E-4</v>
+        <v>-1.1000985109183362E-4</v>
       </c>
     </row>
     <row r="70" spans="1:19" x14ac:dyDescent="0.25">
@@ -21644,7 +23742,7 @@
       </c>
       <c r="S70">
         <f>R70-'No Model 65 MPH'!$Q$20</f>
-        <v>-1.1130243564105429E-4</v>
+        <v>-1.1000985109183362E-4</v>
       </c>
     </row>
     <row r="71" spans="1:19" x14ac:dyDescent="0.25">
@@ -21715,7 +23813,7 @@
       </c>
       <c r="S71">
         <f>R71-'No Model 65 MPH'!$Q$20</f>
-        <v>-8.3800341637786289E-5</v>
+        <v>-8.2507757088565615E-5</v>
       </c>
     </row>
     <row r="72" spans="1:19" x14ac:dyDescent="0.25">
@@ -21786,7 +23884,7 @@
       </c>
       <c r="S72">
         <f>R72-'No Model 65 MPH'!$Q$19</f>
-        <v>1.2610595828125629E-4</v>
+        <v>1.3383650149730353E-4</v>
       </c>
     </row>
     <row r="73" spans="1:19" x14ac:dyDescent="0.25">
@@ -21857,7 +23955,7 @@
       </c>
       <c r="S73">
         <f>R73-'No Model 65 MPH'!$Q$19</f>
-        <v>1.2610595828125629E-4</v>
+        <v>1.3383650149730353E-4</v>
       </c>
     </row>
     <row r="74" spans="1:19" x14ac:dyDescent="0.25">
@@ -21928,7 +24026,7 @@
       </c>
       <c r="S74">
         <f>R74-'No Model 65 MPH'!$Q$19</f>
-        <v>1.2610595828125629E-4</v>
+        <v>1.3383650149730353E-4</v>
       </c>
     </row>
     <row r="75" spans="1:19" x14ac:dyDescent="0.25">
@@ -21999,7 +24097,7 @@
       </c>
       <c r="S75">
         <f>R75-'No Model 65 MPH'!$Q$19</f>
-        <v>1.090055639766524E-4</v>
+        <v>1.1673610719269964E-4</v>
       </c>
     </row>
     <row r="76" spans="1:19" x14ac:dyDescent="0.25">
@@ -22070,7 +24168,7 @@
       </c>
       <c r="S76">
         <f>R76-'No Model 65 MPH'!$Q$20</f>
-        <v>1.0186306351690305E-4</v>
+        <v>1.0315564806612373E-4</v>
       </c>
     </row>
     <row r="77" spans="1:19" x14ac:dyDescent="0.25">
@@ -22125,8 +24223,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q75"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22141,8 +24239,7 @@
     <col min="9" max="10" width="14.7109375" customWidth="1"/>
     <col min="12" max="12" width="12.28515625" customWidth="1"/>
     <col min="14" max="14" width="6" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -22960,8 +25057,8 @@
         <v>3.354726631787215E-5</v>
       </c>
       <c r="Q18">
-        <f>AVERAGE(J61:J65)</f>
-        <v>-2.7852145870460398E-4</v>
+        <f>AVERAGE(J56:J60)</f>
+        <v>-2.4724701494395376E-4</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
@@ -23010,8 +25107,8 @@
         <v>3.1210640803194491E-5</v>
       </c>
       <c r="Q19">
-        <f>AVERAGE(J64:J65)</f>
-        <v>-2.7079091548855674E-4</v>
+        <f>AVERAGE(J61:J65)</f>
+        <v>-2.7852145870460398E-4</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
@@ -23060,8 +25157,8 @@
         <v>3.809534098036974E-5</v>
       </c>
       <c r="Q20">
-        <f>AVERAGE(J67:J70)</f>
-        <v>-2.6364841502880739E-4</v>
+        <f>AVERAGE(J66:J70)</f>
+        <v>-2.6494099957802806E-4</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">

</xml_diff>